<commit_message>
final version with best tuning
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new file\semester5&amp;6\Artificial Intelligence Methods\CW\memetic algorithm\AI_method_memetic_algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD6E99-D690-4649-95AD-72E8B4A4DBF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9662B4-CCD7-4AA1-9B07-20D9010C6188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,8 +1013,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.000000_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1058,12 +1058,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1346,22 +1348,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.86328125" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="3"/>
+    <col min="2" max="2" width="8.06640625" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="3.1328125" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="7.46484375" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
     <col min="14" max="14" width="9.06640625" style="1"/>
+    <col min="15" max="15" width="2.3984375" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="8" customWidth="1"/>
     <col min="19" max="19" width="9.06640625" style="1"/>
+    <col min="20" max="20" width="2.73046875" customWidth="1"/>
+    <col min="22" max="22" width="8.06640625" customWidth="1"/>
+    <col min="23" max="23" width="8.3984375" customWidth="1"/>
     <col min="24" max="24" width="9.06640625" style="1"/>
+    <col min="25" max="25" width="2.73046875" customWidth="1"/>
+    <col min="27" max="28" width="8.19921875" customWidth="1"/>
     <col min="29" max="29" width="9.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="2.6640625" customWidth="1"/>
+    <col min="32" max="32" width="7.86328125" customWidth="1"/>
+    <col min="33" max="33" width="8.19921875" customWidth="1"/>
     <col min="34" max="34" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.3984375" customWidth="1"/>
     <col min="39" max="39" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -1450,7 +1468,7 @@
       <c r="AF1">
         <v>21946</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="6">
         <v>21735</v>
       </c>
       <c r="AH1" s="1">
@@ -1662,7 +1680,7 @@
       <c r="AF3">
         <v>20754</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="5">
         <v>20466</v>
       </c>
       <c r="AH3" s="4">
@@ -2086,7 +2104,7 @@
       <c r="AF7">
         <v>21799</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="6">
         <v>21772</v>
       </c>
       <c r="AH7" s="1">
@@ -2192,7 +2210,7 @@
       <c r="AF8">
         <v>21397</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="5">
         <v>21169</v>
       </c>
       <c r="AH8" s="4">
@@ -2298,7 +2316,7 @@
       <c r="AF9">
         <v>22493</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="6">
         <v>22395</v>
       </c>
       <c r="AH9" s="1">
@@ -2311,7 +2329,7 @@
       <c r="AK9">
         <v>57442</v>
       </c>
-      <c r="AL9">
+      <c r="AL9" s="6">
         <v>57167</v>
       </c>
       <c r="AM9" s="1">

</xml_diff>